<commit_message>
modified sendkeys data from Excel
</commit_message>
<xml_diff>
--- a/src/main/java/com/guru/qa/testdata/Guru99_NewCustomerCreationPage_FRAMEWORK.xlsx
+++ b/src/main/java/com/guru/qa/testdata/Guru99_NewCustomerCreationPage_FRAMEWORK.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="5955" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16080" windowHeight="5955" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="NewCustomers" sheetId="1" r:id="rId1"/>
     <sheet name="NewAccounts" sheetId="2" r:id="rId2"/>
     <sheet name="Deposit" sheetId="3" r:id="rId3"/>
     <sheet name="CustomerIdDataSheet" sheetId="4" r:id="rId4"/>
+    <sheet name="AutoCompleteSampleSheet" sheetId="5" r:id="rId5"/>
+    <sheet name="DataFromSeleniumEasyURL" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
   <si>
     <t>Email</t>
   </si>
@@ -230,6 +231,24 @@
   </si>
   <si>
     <t>49917</t>
+  </si>
+  <si>
+    <t>AutoCompleteValue</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>ChildWindow</t>
+  </si>
+  <si>
+    <t>vishalg@testmail.com</t>
+  </si>
+  <si>
+    <t>datepicker</t>
+  </si>
+  <si>
+    <t>09/10/1968</t>
   </si>
 </sst>
 </file>
@@ -293,13 +312,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -581,7 +601,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
@@ -944,7 +964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -981,4 +1001,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor changes fetching dd values from excel
</commit_message>
<xml_diff>
--- a/src/main/java/com/guru/qa/testdata/Guru99_NewCustomerCreationPage_FRAMEWORK.xlsx
+++ b/src/main/java/com/guru/qa/testdata/Guru99_NewCustomerCreationPage_FRAMEWORK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16080" windowHeight="5955" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16080" windowHeight="5955" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="NewCustomers" sheetId="1" r:id="rId1"/>
@@ -236,9 +236,6 @@
     <t>AutoCompleteValue</t>
   </si>
   <si>
-    <t>java</t>
-  </si>
-  <si>
     <t>ChildWindow</t>
   </si>
   <si>
@@ -249,6 +246,9 @@
   </si>
   <si>
     <t>09/10/1968</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1036,7 +1036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -1048,18 +1048,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done few modifications in TestUtility class
</commit_message>
<xml_diff>
--- a/src/main/java/com/guru/qa/testdata/Guru99_NewCustomerCreationPage_FRAMEWORK.xlsx
+++ b/src/main/java/com/guru/qa/testdata/Guru99_NewCustomerCreationPage_FRAMEWORK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16080" windowHeight="5955" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16080" windowHeight="5955" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="NewCustomers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>Email</t>
   </si>
@@ -222,15 +222,6 @@
   </si>
   <si>
     <t>84433</t>
-  </si>
-  <si>
-    <t>46927</t>
-  </si>
-  <si>
-    <t>95677</t>
-  </si>
-  <si>
-    <t>49917</t>
   </si>
   <si>
     <t>AutoCompleteValue</t>
@@ -607,7 +598,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,10 +956,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,21 +977,6 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1011,27 +987,28 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1056,18 +1033,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added dropdown validation in CommonFunctionUsageTestSelEasy class
</commit_message>
<xml_diff>
--- a/src/main/java/com/guru/qa/testdata/Guru99_NewCustomerCreationPage_FRAMEWORK.xlsx
+++ b/src/main/java/com/guru/qa/testdata/Guru99_NewCustomerCreationPage_FRAMEWORK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16080" windowHeight="5955" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16080" windowHeight="5955" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="NewCustomers" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="CustomerIdDataSheet" sheetId="4" r:id="rId4"/>
     <sheet name="AutoCompleteSampleSheet" sheetId="5" r:id="rId5"/>
     <sheet name="DataFromSeleniumEasyURL" sheetId="8" r:id="rId6"/>
+    <sheet name="DDDataFromSeleniumEasyURL" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>Email</t>
   </si>
@@ -243,6 +244,24 @@
   </si>
   <si>
     <t>Java</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
   </si>
 </sst>
 </file>
@@ -986,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1022,7 +1041,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,4 +1073,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>